<commit_message>
last commit romain windows
</commit_message>
<xml_diff>
--- a/Power-Load_solar_bank.xlsx
+++ b/Power-Load_solar_bank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roco2\Desktop\NanoSat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8558B973-DF88-4C66-905E-FB0333DFC1F0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F964952E-3D0C-49C8-AFC4-BB25E91CCAFE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{3BEC3704-A598-4C4D-9EE9-24BD33A5463B}"/>
   </bookViews>
@@ -1102,6 +1102,21 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D31DFD60-3219-4F5B-B13F-73FD680F0C3C}" name="Tableau1" displayName="Tableau1" ref="A1:D7" totalsRowShown="0">
+  <autoFilter ref="A1:D7" xr:uid="{E371FC09-6689-45D4-AB43-330B8666DE57}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C4E15E1B-012F-48A0-9322-1B7C07AE60EB}" name="Load (kΩ)"/>
+    <tableColumn id="2" xr3:uid="{89E5BE06-4580-49E5-A7B2-583A736E0060}" name="Tension (V)"/>
+    <tableColumn id="3" xr3:uid="{D4B72D31-B529-42F8-A021-E0685E308EDB}" name="Current (mA)"/>
+    <tableColumn id="4" xr3:uid="{AE8E186B-129D-4C45-A3D7-6942301CECEA}" name="Power (mW)">
+      <calculatedColumnFormula>B2*C2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -1402,13 +1417,15 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCellId="1" sqref="L16 A1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1519,5 +1536,8 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>